<commit_message>
Reporte Normativa Plurinacional imp y funcional
</commit_message>
<xml_diff>
--- a/assets/info/plantilla-reportes-normativa-plurinacional.xlsx
+++ b/assets/info/plantilla-reportes-normativa-plurinacional.xlsx
@@ -22,54 +22,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t xml:space="preserve">REPORTE NORMATIVA</t>
   </si>
   <si>
+    <t xml:space="preserve">DATOS DEL REGISTRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATOS GENERALES DEL PROYECTO DE LEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRESENTACIÓN DEL PROYECTO DE LEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULTIMA REPOSICION DEL PROYECTO DE LEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTROS</t>
+  </si>
+  <si>
     <t xml:space="preserve">No</t>
   </si>
   <si>
+    <t xml:space="preserve">FECHA INGRESO INFORMACION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONITOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBSERVACIONES METODOLOGICAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODIGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE DE LA NORMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJETO DE LA NORMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMA 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMA 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROPUESTA POR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUIEN PRESENTA EL PROYECTO DE LEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A QUIEN SE LE PRESENTA EL PROYECTO DE LEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA DE PRESENTACIÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUIEN PRESENTA SOLICITUD DE REPOSICION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A QUIEN SE PRESENTA SOLICITUD DE REPOSICION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA DE SOLICITUD DE REPOSICION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBSERVACIONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENLACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPORTES NOTICIAS</t>
+  </si>
+  <si>
     <t xml:space="preserve">FECHA REGISTRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FECHA PLENARIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSTANCIA DE SEGUIMIENTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEPARTAMENTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUNICIPIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUNTOS DE LA AGENDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CUMPLIMIENTO DE LA AGENDA [%]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESCRIPCION DEL ASUNTO QUE SE DEJO SIN TRATAMIENTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUNTOS VARIOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUMERO Y NOMBRE DE LA NORMA QUE INGRESO SIN ESTAR EN AGENDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIPO DE PLENARIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OBSERVACIONES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MONITOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REPORTES NOTICIAS</t>
   </si>
   <si>
     <t xml:space="preserve">FECHA NOTICIA</t>
@@ -103,7 +133,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -148,6 +178,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
@@ -162,8 +199,16 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +219,36 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4472C4"/>
         <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6E3B6"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC05100"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA766"/>
+        <bgColor rgb="FFFFC499"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD668"/>
+        <bgColor rgb="FFFFC499"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC499"/>
+        <bgColor rgb="FFFCD668"/>
       </patternFill>
     </fill>
   </fills>
@@ -211,7 +286,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -248,16 +323,44 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -308,14 +411,14 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFA6E3B6"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFFA766"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -333,11 +436,11 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFC499"/>
       <rgbColor rgb="FF4472C4"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF93C90F"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFCD668"/>
       <rgbColor rgb="FFEF9600"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -346,7 +449,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC05100"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -362,11 +465,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>66600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>985680</xdr:colOff>
+      <xdr:colOff>984240</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
@@ -381,8 +484,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="66600" y="314640"/>
-          <a:ext cx="3589200" cy="1122120"/>
+          <a:off x="66600" y="316080"/>
+          <a:ext cx="3587760" cy="1120680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -408,9 +511,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>919080</xdr:colOff>
+      <xdr:colOff>917640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>179280</xdr:rowOff>
+      <xdr:rowOff>177840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -424,7 +527,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="313920"/>
-          <a:ext cx="3522600" cy="1255680"/>
+          <a:ext cx="3521160" cy="1254240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -450,9 +553,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>726840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>226800</xdr:rowOff>
+      <xdr:rowOff>225360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -466,7 +569,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="313920"/>
-          <a:ext cx="3331800" cy="1303200"/>
+          <a:ext cx="3330360" cy="1301760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -486,30 +589,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q6" activeCellId="0" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="46.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="59.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="43.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="44.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="37.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="34.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="28.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="29.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="34.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="43.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="57.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="37.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="41.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="40.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="37.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="40.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="37.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="4" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="32.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="4" width="34.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="4" width="32.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="19" style="4" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -541,58 +647,109 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="R5" s="13"/>
+    </row>
+    <row r="6" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="B6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="C6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="D6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="E6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="F6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="G6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="H6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="I6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="10"/>
+      <c r="J6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="17"/>
+      <c r="K7" s="18"/>
+      <c r="N7" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:R5"/>
   </mergeCells>
-  <conditionalFormatting sqref="G6:G1048576">
+  <conditionalFormatting sqref="G7:G1048576">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Reforma Electoral" dxfId="0">
-      <formula>NOT(ISERROR(SEARCH("Reforma Electoral",G6)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Reforma Electoral",G7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
@@ -600,12 +757,12 @@
       <formula>NOT(ISERROR(SEARCH("Reforma Electoral",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G1048576 G1:G4 H5">
+  <conditionalFormatting sqref="G7:G1048576 G1:G5 H6">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Censo" dxfId="1">
       <formula>NOT(ISERROR(SEARCH("Censo",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G1048576 G1:G4 H5">
+  <conditionalFormatting sqref="G7:G1048576 G1:G5 H6">
     <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Institucionalidad Democratica" dxfId="2">
       <formula>NOT(ISERROR(SEARCH("Institucionalidad Democratica",G1)))</formula>
     </cfRule>
@@ -654,7 +811,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -682,37 +839,37 @@
       <c r="F4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="A5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -782,7 +939,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -810,39 +967,39 @@
       <c r="F4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="A5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>